<commit_message>
Updated main script and DB functions
</commit_message>
<xml_diff>
--- a/testing/BleepingComputer/BleepingComputer.xlsx
+++ b/testing/BleepingComputer/BleepingComputer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1432,6 +1432,357 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Ivanti Avalanche impacted by critical pre-auth stack buffer overflows</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/ivanti-avalanche-impacted-by-critical-pre-auth-stack-buffer-overflows/</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Two stack-based buffer overflows collectively tracked as CVE-2023-32560 impact Ivanti Avalanche, an enterprise mobility management (EMM) solution designed to manage, monitor, and secure a wide range of mobile devices. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>LinkedIn accounts hacked in widespread hijacking campaign</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/linkedin-accounts-hacked-in-widespread-hijacking-campaign/</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>LinkedIn is being targeted in a wave of account hacks resulting in many accounts being locked out for security reasons or ultimately hijacked by attackers. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Almost 2,000 Citrix NetScaler servers backdoored in hacking campaign</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/almost-2-000-citrix-netscaler-servers-backdoored-in-hacking-campaign/</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>A threat actor has compromised close to 2,000 thousand Citrix NetScaler servers in a massive campaign exploiting the critical-severity remote code execution tracked as CVE-2023-3519. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Raccoon Stealer malware returns with new stealthier version</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/raccoon-stealer-malware-returns-with-new-stealthier-version/</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>The developers of Raccoon Stealer information-stealing malware have ended their 6-month hiatus from hacker forums to promote a new 2.3.0 version of the malware to cyber criminals. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>New CVE-2023-3519 scanner detects hacked Citrix ADC, Gateway devices</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/new-cve-2023-3519-scanner-detects-hacked-citrix-adc-gateway-devices/</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Mandiant has released a scanner to check if a Citrix NetScaler Application Delivery Controller (ADC) or NetScaler Gateway Appliance was compromised in widespread attacks exploiting the CVE-2023-3519 vulnerability.  [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Back to school security against ransomware attacks on K-12 and colleges</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/back-to-school-security-against-ransomware-attacks-on-k-12-and-colleges/</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2023-08-15</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>As we get back to school, K-12 and colleges are increasingly at risk from ransomware and data theft attacks. Learn more from Specops Software on the steps IT teams at education institutes can take to protect their care orgs from disruption and stolen data. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Threat actors use beta apps to bypass mobile app store security</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/threat-actors-use-beta-apps-to-bypass-mobile-app-store-security/</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>The FBI is warning of a new tactic used by cybercriminals where they promote malicious beta versions of cryptocurrency investment apps on popular mobile app stores that are then used to steal crypto. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Discord.io confirms breach after hacker steals data of 760K users</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/discordio-confirms-breach-after-hacker-steals-data-of-760k-users/</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>The Discord.io custom invite service has temporarily shut down after suffering a data breach exposing the information of 760,000 members. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Over 100K hacking forums accounts exposed by info-stealing malware</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/over-100k-hacking-forums-accounts-exposed-by-info-stealing-malware/</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Researchers discovered 120,000 infected systems that contained credentials for cybercrime forums. Many of the computers belong to hackers, the researchers say. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Microsoft enables Windows Kernel CVE-2023-32019 fix for everyone</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/microsoft/microsoft-enables-windows-kernel-cve-2023-32019-fix-for-everyone/</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Microsoft has enabled a fix for a Kernel information disclosure vulnerability by default for everyone after previously disabling it out of concerns it could introduce breaking changes to Windows. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>FBI warns of increasing cryptocurrency recovery scams</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/fbi-warns-of-increasing-cryptocurrency-recovery-scams/</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>The FBI is warning of an increase in scammers pretending to be recovery companies that can help victims of cryptocurrency investment scams recover lost assets. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Monti ransomware targets VMware ESXi servers with new Linux locker</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/monti-ransomware-targets-vmware-esxi-servers-with-new-linux-locker/</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>The Monti ransomware has returned to action after a two-month hiatus, now targeting primarily legal and government organizations, and VMware ESXi servers using a new Linux variant that is vastly different from its predecessors. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Criminal IP Teams Up with PolySwarm to Strengthen Threat Detection</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/criminal-ip-teams-up-with-polyswarm-to-strengthen-threat-detection/</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2023-08-14</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>The addition of Criminal IP as a new contributor to PolySwarm's malicious URL detection represents a significant leap in specialized threat identification. Learn more from Criminal IP about this new collaboration. [...]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added bash script for automation
</commit_message>
<xml_diff>
--- a/testing/BleepingComputer/BleepingComputer.xlsx
+++ b/testing/BleepingComputer/BleepingComputer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1783,6 +1783,330 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Hands on with Windows 11's 'never combine' taskbar feature</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/microsoft/hands-on-with-windows-11s-never-combine-taskbar-feature/</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2023-08-20</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>In its upcoming 23H2 release slated for fall, one of the standout features that has caught the eye of many is the 'never combine mode' for the taskbar. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Google Chrome to warn when installed extensions are malware</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/google/google-chrome-to-warn-when-installed-extensions-are-malware/</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2023-08-20</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Google is testing a new feature in the Chrome browser that will warn users when an installed extension has been removed from the Chrome Web Store, usually indicative of it being malware. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Cuba ransomware uses Veeam exploit against critical U.S. organizations</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/cuba-ransomware-uses-veeam-exploit-against-critical-us-organizations/</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2023-08-20</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>The Cuba ransomware gang was observed in attacks targeting critical infrastructure organizations in the United States and IT firms in Latin America, using a combination of old and new tools. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Hackers use VPN provider's code certificate to sign malware</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/hackers-use-vpn-providers-code-certificate-to-sign-malware/</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2023-08-19</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>The China-aligned APT (advanced persistent threat) group known as 'Bronze Starlight' was seen targeting the Southeast Asian gambling industry with malware signed using a valid certificate used by the Ivacy VPN provider. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Rust devs push back as Serde project ships precompiled binaries</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/rust-devs-push-back-as-serde-project-ships-precompiled-binaries/</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2023-08-19</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Serde, a popular Rust (de)serialization project, has decided to ship its serde_derive macro as a precompiled binary. This has generated a fair amount of concern among some developers who highlight the future legal and technical issues this may pose, along with a potential for supply chain attacks. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>The Week in Ransomware - August 18th 2023 - LockBit on Thin Ice</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/the-week-in-ransomware-august-18th-2023-lockbit-on-thin-ice/</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2023-08-18</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>While there was quite a bit of ransomware news this week, the highlighted story was the release of Jon DiMaggio's third article in the Ransomware Diaries series, with the focus of this article on the LockBit ransomware operation. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>WinRAR flaw lets hackers run programs when you open RAR archives</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/winrar-flaw-lets-hackers-run-programs-when-you-open-rar-archives/</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2023-08-18</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>A high-severity vulnerability has been fixed in WinRAR, the popular file archiver utility for Windows used by millions, that can execute commands on a computer simply by opening an archive. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Hotmail email delivery fails after Microsoft misconfigures DNS</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/microsoft/hotmail-email-delivery-fails-after-microsoft-misconfigures-dns/</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2023-08-18</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Hotmail users worldwide have problems sending emails, with messages flagged as spam or not delivered after Microsoft misconfigured the domain's DNS SPF record. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Interpol arrests 14 suspected cybercriminals for stealing $40 million</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/interpol-arrests-14-suspected-cybercriminals-for-stealing-40-million/</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2023-08-18</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>An international law enforcement operation led by Interpol has led to the arrest of 14 suspected cybercriminals in an operation codenamed 'Africa Cyber Surge II,' launched in April 2023. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Microsoft: BlackCat's Sphynx ransomware embeds Impacket, RemCom</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/microsoft/microsoft-blackcats-sphynx-ransomware-embeds-impacket-remcom/</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2023-08-17</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Microsoft has discovered a new version of the BlackCat ransomware that embeds the Impacket networking framework and the Remcom hacking tool, both enabling spreading laterally across a breached network. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Hackers ask $120,000 for access to multi-billion auction house</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/hackers-ask-120-000-for-access-to-multi-billion-auction-house/</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2023-08-17</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Hackers have breached the network of a major auction house and offered access to whoever was willing to pay $120,000. [...]</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Microsoft PowerShell Gallery vulnerable to spoofing, supply chain attacks</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/security/microsoft-powershell-gallery-vulnerable-to-spoofing-supply-chain-attacks/</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2023-08-17</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Lax policies for package naming on Microsoft's PowerShell Gallery code repository allow threat actors to perform typosquatting attacks, spoof popular packages and potentially lay the ground for massive supply chain attacks. [...]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bash syntax and other bugs in main script
</commit_message>
<xml_diff>
--- a/testing/BleepingComputer/BleepingComputer.xlsx
+++ b/testing/BleepingComputer/BleepingComputer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2161,6 +2161,33 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>BleepingComputer</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Ongoing Duo outage causes Azure Auth authentication errors</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://www.bleepingcomputer.com/news/technology/ongoing-duo-outage-causes-azure-auth-authentication-errors/</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2023-08-21</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Cisco-owned multi-factor authentication (MFA) provider Duo Security is investigating an ongoing outage that has been causing authentication failures and errors starting three hours ago. [...]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Fixed bash syntax and other bugs in main script"
This reverts commit 78d61db60c70cec0161a1d3d8254e727e79b537a.
</commit_message>
<xml_diff>
--- a/testing/BleepingComputer/BleepingComputer.xlsx
+++ b/testing/BleepingComputer/BleepingComputer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2161,33 +2161,6 @@
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>BleepingComputer</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Ongoing Duo outage causes Azure Auth authentication errors</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>https://www.bleepingcomputer.com/news/technology/ongoing-duo-outage-causes-azure-auth-authentication-errors/</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>2023-08-21</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>Cisco-owned multi-factor authentication (MFA) provider Duo Security is investigating an ongoing outage that has been causing authentication failures and errors starting three hours ago. [...]</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>